<commit_message>
modified:   massen_gesamt.xlsx 	modified:   massen_haltungen.csv 	modified:   massen_util/merge_elements.py 	deleted:    massen_util/src/.~lock.massen.xlsx#
</commit_message>
<xml_diff>
--- a/massen_gesamt.xlsx
+++ b/massen_gesamt.xlsx
@@ -2930,7 +2930,7 @@
         <v>208.41</v>
       </c>
       <c r="D17" s="115" t="n">
-        <v>0</v>
+        <v>206.47</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>206.664</v>
@@ -4664,7 +4664,7 @@
         <v>215.21</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>211.63</v>
       </c>
       <c r="E46" t="n">
         <v>213.119</v>
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>211.63</v>
       </c>
       <c r="D47" t="n">
         <v>213.67</v>

</xml_diff>

<commit_message>
modified:   input/Stammdaten_ISY.xml 	modified:   main.py 	modified:   massen_gesamt.xlsx 	modified:   massen_haltungen.csv 	deleted:    massen_haltungen.xlsx 	modified:   requirements.txt
</commit_message>
<xml_diff>
--- a/massen_gesamt.xlsx
+++ b/massen_gesamt.xlsx
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B32" s="133" t="inlineStr">
         <is>
-          <t>24_R�</t>
+          <t>24_Rï¿½</t>
         </is>
       </c>
       <c r="C32" s="134" t="n">
@@ -4232,12 +4232,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>HS-027</t>
+          <t>H-026</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>H-026</t>
+          <t>H-025</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -4247,16 +4247,16 @@
         <v>206.83</v>
       </c>
       <c r="E34" t="n">
-        <v>204.59</v>
+        <v>203.76</v>
       </c>
       <c r="F34" t="n">
-        <v>204.26</v>
+        <v>203.74</v>
       </c>
       <c r="G34" t="n">
-        <v>52.42</v>
+        <v>4</v>
       </c>
       <c r="L34" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="W34" t="inlineStr">
         <is>
@@ -4267,12 +4267,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>HS-027</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>H-026</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>H-025</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -4282,16 +4282,16 @@
         <v>206.83</v>
       </c>
       <c r="E35" t="n">
-        <v>203.76</v>
+        <v>204.59</v>
       </c>
       <c r="F35" t="n">
-        <v>203.74</v>
+        <v>204.26</v>
       </c>
       <c r="G35" t="n">
-        <v>4</v>
+        <v>52.42</v>
       </c>
       <c r="L35" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="W35" t="inlineStr">
         <is>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>W_R�</t>
+          <t>W_Rï¿½</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -6857,7 +6857,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>24_R�</t>
+          <t>24_Rï¿½</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -7032,28 +7032,28 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>748</t>
+          <t>747</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>747</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>207.95</v>
+        <v>207.92</v>
       </c>
       <c r="D114" t="n">
-        <v>207.92</v>
+        <v>209.55</v>
       </c>
       <c r="E114" t="n">
-        <v>206.97</v>
+        <v>205.929</v>
       </c>
       <c r="F114" t="n">
-        <v>206.59</v>
+        <v>205.761</v>
       </c>
       <c r="G114" t="n">
-        <v>1.36</v>
+        <v>62.01</v>
       </c>
       <c r="L114" t="n">
         <v>300</v>
@@ -7067,28 +7067,28 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>748</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>747</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>746</t>
-        </is>
-      </c>
       <c r="C115" t="n">
+        <v>207.95</v>
+      </c>
+      <c r="D115" t="n">
         <v>207.92</v>
       </c>
-      <c r="D115" t="n">
-        <v>209.55</v>
-      </c>
       <c r="E115" t="n">
-        <v>205.929</v>
+        <v>206.97</v>
       </c>
       <c r="F115" t="n">
-        <v>205.761</v>
+        <v>206.59</v>
       </c>
       <c r="G115" t="n">
-        <v>62.01</v>
+        <v>1.36</v>
       </c>
       <c r="L115" t="n">
         <v>300</v>

</xml_diff>

<commit_message>
modified:   main.py 	modified:   massen_gesamt.xlsx 	modified:   massen_haltungen.csv 	modified:   massen_schacht.csv 	modified:   xml_parser/__init__.py 	modified:   xml_parser/xml_fixer.py
</commit_message>
<xml_diff>
--- a/massen_gesamt.xlsx
+++ b/massen_gesamt.xlsx
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B32" s="133" t="inlineStr">
         <is>
-          <t>24_Rï¿½</t>
+          <t>24_R_</t>
         </is>
       </c>
       <c r="C32" s="134" t="n">
@@ -5392,7 +5392,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>W_Rï¿½</t>
+          <t>W_R_</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -6857,7 +6857,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>24_Rï¿½</t>
+          <t>24_R_</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -8531,7 +8531,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>W_Rï¿½</t>
+          <t>W_R_</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -9027,7 +9027,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>24_Rï¿½</t>
+          <t>24_R_</t>
         </is>
       </c>
       <c r="B88" t="n">

</xml_diff>

<commit_message>
modified:   input/Stammdaten_ISY.xml 	modified:   main.py 	modified:   massen_gesamt.xlsx 	modified:   massen_haltungen.csv 	modified:   massen_schacht.csv 	modified:   massen_util/merge_elements.py 	modified:   xml_parser/__init__.py 	modified:   xml_parser/haltung.py 	modified:   xml_parser/xml_fixer.py
</commit_message>
<xml_diff>
--- a/massen_gesamt.xlsx
+++ b/massen_gesamt.xlsx
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B32" s="133" t="inlineStr">
         <is>
-          <t>24_R_</t>
+          <t>24_RUe</t>
         </is>
       </c>
       <c r="C32" s="134" t="n">
@@ -5392,7 +5392,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>W_R_</t>
+          <t>W_RUe</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -6857,7 +6857,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>24_R_</t>
+          <t>24_RUe</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -8531,7 +8531,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>W_R_</t>
+          <t>W_RUe</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -9027,7 +9027,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>24_R_</t>
+          <t>24_RUe</t>
         </is>
       </c>
       <c r="B88" t="n">

</xml_diff>